<commit_message>
uploaded working source code
</commit_message>
<xml_diff>
--- a/Xlsx/UserStories.xlsx
+++ b/Xlsx/UserStories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemanvithamylapalli/Documents/GitHub/2024S-neon-nomads/Xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemanvithamylapalli/Desktop/2024S-neon-nomads/Xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F439ADCE-E5CA-F54B-9E02-FB06A491E2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435AAD7E-C1E4-DA4B-877C-95CF55A45753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17040" xr2:uid="{B14A5D20-9606-4AFA-A377-67AB9C52EFC1}"/>
   </bookViews>
@@ -74,30 +74,9 @@
     <t>Estimation</t>
   </si>
   <si>
-    <t xml:space="preserve">track my food expense </t>
-  </si>
-  <si>
-    <t>I can manage my budget more effectively</t>
-  </si>
-  <si>
     <t>Feature</t>
   </si>
   <si>
-    <t>Expense Tracking</t>
-  </si>
-  <si>
-    <t>Busy Parent</t>
-  </si>
-  <si>
-    <t>I can automatically update my pantry inventory</t>
-  </si>
-  <si>
-    <t>easily upload my grocery receipts</t>
-  </si>
-  <si>
-    <t>Receipt Upload</t>
-  </si>
-  <si>
     <t>Health-conscious Individual</t>
   </si>
   <si>
@@ -155,9 +134,6 @@
     <t xml:space="preserve">College Student </t>
   </si>
   <si>
-    <t>Student on a budget</t>
-  </si>
-  <si>
     <t>find recipes based on the ingredients I have</t>
   </si>
   <si>
@@ -255,6 +231,30 @@
   </si>
   <si>
     <t>I can keep track of what I have</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student </t>
+  </si>
+  <si>
+    <t>upload an image of food</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>see detailed nutritional information for the food in the uploaded image</t>
+  </si>
+  <si>
+    <t>I can make informed dietary choices</t>
+  </si>
+  <si>
+    <t>I can receive video recipes related to the image</t>
+  </si>
+  <si>
+    <t>Nutritional Analysis</t>
+  </si>
+  <si>
+    <t>Recipe Recommendation</t>
   </si>
 </sst>
 </file>
@@ -710,8 +710,8 @@
   </sheetPr>
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -742,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>4</v>
@@ -759,16 +759,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>10</v>
@@ -785,16 +785,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>10</v>
@@ -811,22 +811,22 @@
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -837,16 +837,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>10</v>
@@ -863,22 +863,22 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -889,22 +889,22 @@
         <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -915,22 +915,22 @@
         <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -941,16 +941,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>10</v>
@@ -967,22 +967,22 @@
         <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -996,19 +996,19 @@
         <v>6</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1019,16 +1019,16 @@
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>10</v>
@@ -1037,7 +1037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="6" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>3</v>
       </c>
@@ -1045,16 +1045,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>10</v>
@@ -1071,22 +1071,22 @@
         <v>13</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1097,22 +1097,22 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1123,22 +1123,22 @@
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1149,16 +1149,16 @@
         <v>16</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>10</v>
@@ -1175,16 +1175,16 @@
         <v>17</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>10</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="20" spans="1:8" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
65y iMerge branch 'main' of https://github.com/htmw/2024S-neon-nomads into Sasank
</commit_message>
<xml_diff>
--- a/Xlsx/UserStories.xlsx
+++ b/Xlsx/UserStories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemanvithamylapalli/Documents/GitHub/2024S-neon-nomads/Xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemanvithamylapalli/Desktop/2024S-neon-nomads/Xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F439ADCE-E5CA-F54B-9E02-FB06A491E2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435AAD7E-C1E4-DA4B-877C-95CF55A45753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17040" xr2:uid="{B14A5D20-9606-4AFA-A377-67AB9C52EFC1}"/>
   </bookViews>
@@ -74,30 +74,9 @@
     <t>Estimation</t>
   </si>
   <si>
-    <t xml:space="preserve">track my food expense </t>
-  </si>
-  <si>
-    <t>I can manage my budget more effectively</t>
-  </si>
-  <si>
     <t>Feature</t>
   </si>
   <si>
-    <t>Expense Tracking</t>
-  </si>
-  <si>
-    <t>Busy Parent</t>
-  </si>
-  <si>
-    <t>I can automatically update my pantry inventory</t>
-  </si>
-  <si>
-    <t>easily upload my grocery receipts</t>
-  </si>
-  <si>
-    <t>Receipt Upload</t>
-  </si>
-  <si>
     <t>Health-conscious Individual</t>
   </si>
   <si>
@@ -155,9 +134,6 @@
     <t xml:space="preserve">College Student </t>
   </si>
   <si>
-    <t>Student on a budget</t>
-  </si>
-  <si>
     <t>find recipes based on the ingredients I have</t>
   </si>
   <si>
@@ -255,6 +231,30 @@
   </si>
   <si>
     <t>I can keep track of what I have</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student </t>
+  </si>
+  <si>
+    <t>upload an image of food</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>see detailed nutritional information for the food in the uploaded image</t>
+  </si>
+  <si>
+    <t>I can make informed dietary choices</t>
+  </si>
+  <si>
+    <t>I can receive video recipes related to the image</t>
+  </si>
+  <si>
+    <t>Nutritional Analysis</t>
+  </si>
+  <si>
+    <t>Recipe Recommendation</t>
   </si>
 </sst>
 </file>
@@ -710,8 +710,8 @@
   </sheetPr>
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -742,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>4</v>
@@ -759,16 +759,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>10</v>
@@ -785,16 +785,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>10</v>
@@ -811,22 +811,22 @@
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -837,16 +837,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>10</v>
@@ -863,22 +863,22 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -889,22 +889,22 @@
         <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -915,22 +915,22 @@
         <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -941,16 +941,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>10</v>
@@ -967,22 +967,22 @@
         <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -996,19 +996,19 @@
         <v>6</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1019,16 +1019,16 @@
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>10</v>
@@ -1037,7 +1037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="6" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>3</v>
       </c>
@@ -1045,16 +1045,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>10</v>
@@ -1071,22 +1071,22 @@
         <v>13</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1097,22 +1097,22 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1123,22 +1123,22 @@
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1149,16 +1149,16 @@
         <v>16</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>10</v>
@@ -1175,16 +1175,16 @@
         <v>17</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>10</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="20" spans="1:8" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">

</xml_diff>